<commit_message>
markov case study nearly complete 2024-06-14
</commit_message>
<xml_diff>
--- a/case-studies/normalization-for-heterogeneous-effects.xlsx
+++ b/case-studies/normalization-for-heterogeneous-effects.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johngraves/Dropbox/teaching/bogota-vital-strategies/case-studies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D7D2BD9-4457-6F46-862F-E3C8DFB0CF73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677637FD-0B8E-3240-9CEE-B79E008F48CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="500" windowWidth="25600" windowHeight="26740" xr2:uid="{E00F29A5-A747-704C-ADE7-298C5BED839F}"/>
+    <workbookView xWindow="-33080" yWindow="760" windowWidth="31440" windowHeight="21280" xr2:uid="{E00F29A5-A747-704C-ADE7-298C5BED839F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>p_injury</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>rr_fatality_ban</t>
-  </si>
-  <si>
-    <t>1-p_severe</t>
   </si>
   <si>
     <t>p_fatality_ban_</t>
@@ -472,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{399E7ED4-F483-7740-BE90-98B0AB3C9BD2}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="273" zoomScaleNormal="273" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="273" zoomScaleNormal="273" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -513,15 +510,15 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -529,91 +526,85 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8">
-        <f>1-p_severe</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10">
         <f>p_injury*p_fatality*rr_fatality_ban</f>
-        <v>8.0591999999999998E-8</v>
+        <v>1.2088800000000002E-7</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11">
         <f>p_injury*(1-p_fatality*rr_fatality_ban)*p_severe*rr_severe_ban</f>
-        <v>8.1534342400000011E-6</v>
+        <v>1.6284302719999999E-5</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12">
         <f>p_injury*(1-p_fatality*rr_fatality_ban)*((1-p_severe)*rr_mildmod_ban)</f>
-        <v>6.988657920000002E-6</v>
+        <v>6.1066135200000009E-6</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <f>p_fatality_ban_+p_severe_ban_+p_mildmod_ban_</f>
-        <v>1.5222684160000003E-5</v>
+        <v>2.251180424E-5</v>
       </c>
       <c r="C13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14">
         <f>p_severe_ban_/(p_severe_ban_+p_mildmod_ban_)</f>
-        <v>0.53846153846153844</v>
+        <v>0.72727272727272729</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B15">
         <f>p_mildmod_ban_ / (p_severe_ban_+p_mildmod_ban_)</f>
-        <v>0.46153846153846156</v>
+        <v>0.27272727272727276</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <f>B13/p_injury</f>
+        <v>0.77095219999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>